<commit_message>
greenwald meta reproduction updated
</commit_message>
<xml_diff>
--- a/Greenwald & Lai 2020 meta analysis/data/raw_metadataset.xlsx
+++ b/Greenwald & Lai 2020 meta analysis/data/raw_metadataset.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-reliability-meta-analysis/Greenwald &amp; Lai 2020 meta analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFB55BB-235A-094F-8AF2-EA1800FE6AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ACFE13-2484-F84F-BF37-1FCE8383F8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23480" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23480" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="irap" sheetId="11" r:id="rId1"/>
     <sheet name="IRAP Ns" sheetId="13" r:id="rId2"/>
-    <sheet name="iat trt" sheetId="12" r:id="rId3"/>
-    <sheet name="Raw Data" sheetId="10" r:id="rId4"/>
+    <sheet name="iat trt (2)" sheetId="14" r:id="rId3"/>
+    <sheet name="iat trt" sheetId="12" r:id="rId4"/>
+    <sheet name="Raw Data" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -433,6 +434,288 @@
     <author>Calvin Lai</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{138F22C7-22C1-294B-BCC6-33906B448C57}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>APA-style citation of paper</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D1BF3C3B-0D56-AA41-9594-9BA89193A76D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Study number as it's listed within the paper. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{314D2507-4A65-254F-9E69-6F7F6E14EF28}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifier distinguishing the independent samples within a study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2B8FD07A-2EED-3D44-BD65-95C8E7ACAAF9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of the implicit measure</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>examined</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9289BAC7-4272-1E46-B4CB-4A1019977FC0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of estimate retrieved IC = Internal Consistency
+TRR = Test-Retest Reliability</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{650776BA-A970-4743-A9F9-687431ECEC24}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of participants in the analysis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C157B1F2-A2DF-D747-91FF-E5C5EDC74682}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Numerical estimate of reliability</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{A8FFE531-0778-EE49-AC66-7F98B34CFF33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calvin Lai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If only a split-half estimate is provided, list the estimate before it is converted</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{6FD94D86-6E2A-1F4F-BB2A-02930A8961C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calvin Lai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The number of items contributing to the IC estimate. If that information isn't provided, assume it is 2 parts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3CECEE83-05D7-0145-ACF8-1FFC1F3F5825}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calvin Lai:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If the number of items contributing to the alpha estimate are not provided, write "No".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{991B71F8-171F-3345-AD2F-661301C1A6D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>For TRR estimates, time between administrations of the measure</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{1CF96675-B4D7-D649-B47A-09B02B613910}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If estimate is aggregated, describe how it's aggregated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{63808E59-D95B-9C43-9D76-5DF892F7948D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If estimate is aggregated, # of estimates that contributed to the aggregate estimate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{5C281F9B-04E8-B944-83BB-098B8C869665}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Notes detailing what estimates were retrieved (if there are multiple estimates)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{DBC2F4D4-3A89-9B49-BC2D-E9AF7856AE7D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is this estimate directly retrievable from the paper's main text? (Yes/No)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{5F8D69A0-4B3C-3A45-8356-B8F8EEF54607}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Calvin Lai 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Where the data came from (Search = Scopus Search, OrigPub = Definitive early publication, Author = Correspondence with original authors, Review = major psychometric reviews)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Calvin Lai</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7A0672CF-3119-1A4E-AB7C-95D05677099C}">
       <text>
         <r>
@@ -709,7 +992,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Calvin Lai</author>
@@ -992,7 +1275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6733" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7137" uniqueCount="620">
   <si>
     <t>IC</t>
   </si>
@@ -4432,7 +4715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94664F9-5C2C-DB44-8023-011B6DCF3D45}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -4905,11 +5188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78366DC7-9A39-E24B-AC3B-88802F01F8CB}">
-  <dimension ref="A1:P318"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D7BEF3-9CE0-F548-8F66-718CEC57849C}">
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="G319" sqref="G319"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4995,6 +5278,2129 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>39</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>39</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
+        <v>105</v>
+      </c>
+      <c r="P5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>118</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>116</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="K7" t="s">
+        <v>372</v>
+      </c>
+      <c r="N7" t="s">
+        <v>450</v>
+      </c>
+      <c r="O7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>116</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="K8" t="s">
+        <v>372</v>
+      </c>
+      <c r="N8" t="s">
+        <v>452</v>
+      </c>
+      <c r="O8" t="s">
+        <v>105</v>
+      </c>
+      <c r="P8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>116</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="K9" t="s">
+        <v>372</v>
+      </c>
+      <c r="N9" t="s">
+        <v>453</v>
+      </c>
+      <c r="O9" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>67</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="K10" t="s">
+        <v>372</v>
+      </c>
+      <c r="N10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>67</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="K11" t="s">
+        <v>372</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>78</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="K12" t="s">
+        <v>139</v>
+      </c>
+      <c r="O12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>87</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="K13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O13" t="s">
+        <v>105</v>
+      </c>
+      <c r="P13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>102</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="K14" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>195</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>110</v>
+      </c>
+      <c r="O15" t="s">
+        <v>105</v>
+      </c>
+      <c r="P15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>94</v>
+      </c>
+      <c r="G16">
+        <v>0.34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>136</v>
+      </c>
+      <c r="N16" t="s">
+        <v>132</v>
+      </c>
+      <c r="O16" t="s">
+        <v>105</v>
+      </c>
+      <c r="P16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>74</v>
+      </c>
+      <c r="G17">
+        <v>0.48</v>
+      </c>
+      <c r="K17" t="s">
+        <v>136</v>
+      </c>
+      <c r="N17" t="s">
+        <v>133</v>
+      </c>
+      <c r="O17" t="s">
+        <v>105</v>
+      </c>
+      <c r="P17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>60</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="K18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>141</v>
+      </c>
+      <c r="O18" t="s">
+        <v>105</v>
+      </c>
+      <c r="P18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>61</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" t="s">
+        <v>142</v>
+      </c>
+      <c r="O19" t="s">
+        <v>105</v>
+      </c>
+      <c r="P19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" t="s">
+        <v>143</v>
+      </c>
+      <c r="O20" t="s">
+        <v>105</v>
+      </c>
+      <c r="P20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>54</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="K21" t="s">
+        <v>178</v>
+      </c>
+      <c r="N21" t="s">
+        <v>145</v>
+      </c>
+      <c r="O21" t="s">
+        <v>105</v>
+      </c>
+      <c r="P21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>93</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="K22" t="s">
+        <v>578</v>
+      </c>
+      <c r="N22" t="s">
+        <v>566</v>
+      </c>
+      <c r="O22" t="s">
+        <v>105</v>
+      </c>
+      <c r="P22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>211</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>93</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="K23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" t="s">
+        <v>567</v>
+      </c>
+      <c r="O23" t="s">
+        <v>105</v>
+      </c>
+      <c r="P23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>93</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="K24" t="s">
+        <v>579</v>
+      </c>
+      <c r="N24" t="s">
+        <v>568</v>
+      </c>
+      <c r="O24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>93</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="K25" t="s">
+        <v>578</v>
+      </c>
+      <c r="N25" t="s">
+        <v>569</v>
+      </c>
+      <c r="O25" t="s">
+        <v>105</v>
+      </c>
+      <c r="P25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>93</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="K26" t="s">
+        <v>5</v>
+      </c>
+      <c r="N26" t="s">
+        <v>570</v>
+      </c>
+      <c r="O26" t="s">
+        <v>105</v>
+      </c>
+      <c r="P26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>93</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="K27" t="s">
+        <v>578</v>
+      </c>
+      <c r="N27" t="s">
+        <v>571</v>
+      </c>
+      <c r="O27" t="s">
+        <v>105</v>
+      </c>
+      <c r="P27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>90</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="K28" t="s">
+        <v>372</v>
+      </c>
+      <c r="O28" t="s">
+        <v>105</v>
+      </c>
+      <c r="P28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>913</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="K29" t="s">
+        <v>231</v>
+      </c>
+      <c r="N29" t="s">
+        <v>232</v>
+      </c>
+      <c r="O29" t="s">
+        <v>105</v>
+      </c>
+      <c r="P29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>261</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>101</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="K30" t="s">
+        <v>373</v>
+      </c>
+      <c r="N30" t="s">
+        <v>262</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>261</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <f>98</f>
+        <v>98</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="K31" t="s">
+        <v>263</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>261</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>98</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="K32" t="s">
+        <v>373</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>90</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="K33" t="s">
+        <v>263</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P33" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>88</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="K34" t="s">
+        <v>264</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P34" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>47</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="K35" t="s">
+        <v>374</v>
+      </c>
+      <c r="N35" t="s">
+        <v>281</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>280</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>47</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="K36" t="s">
+        <v>374</v>
+      </c>
+      <c r="N36" t="s">
+        <v>282</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P36" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>46</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="K37" t="s">
+        <v>374</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>344</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="K38" t="s">
+        <v>9</v>
+      </c>
+      <c r="N38" t="s">
+        <v>284</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P38" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>283</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>344</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="K39" t="s">
+        <v>9</v>
+      </c>
+      <c r="N39" t="s">
+        <v>285</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>105</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="H40" s="3"/>
+      <c r="K40" t="s">
+        <v>299</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>305</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>59</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="K41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
+        <v>306</v>
+      </c>
+      <c r="O41" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P41" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>305</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>59</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="K42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" t="s">
+        <v>307</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P42" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>31</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="K43" t="s">
+        <v>316</v>
+      </c>
+      <c r="O43" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P43" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>319</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>93</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="K44" t="s">
+        <v>263</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>341</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>30</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.432</v>
+      </c>
+      <c r="H45" s="3"/>
+      <c r="K45" t="s">
+        <v>342</v>
+      </c>
+      <c r="N45" t="s">
+        <v>343</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P45" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>341</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>30</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="K46" t="s">
+        <v>342</v>
+      </c>
+      <c r="N46" t="s">
+        <v>344</v>
+      </c>
+      <c r="O46" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P46" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>353</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>65</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H47" s="3"/>
+      <c r="K47" t="s">
+        <v>9</v>
+      </c>
+      <c r="N47" t="s">
+        <v>355</v>
+      </c>
+      <c r="O47" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>353</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>39</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="K48" t="s">
+        <v>263</v>
+      </c>
+      <c r="N48" t="s">
+        <v>355</v>
+      </c>
+      <c r="O48" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P48" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>353</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>36</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="H49" s="3"/>
+      <c r="K49" t="s">
+        <v>264</v>
+      </c>
+      <c r="N49" t="s">
+        <v>355</v>
+      </c>
+      <c r="O49" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P49" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>356</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>90</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="K50" t="s">
+        <v>357</v>
+      </c>
+      <c r="N50" t="s">
+        <v>358</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P50" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>356</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>90</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="K51" t="s">
+        <v>357</v>
+      </c>
+      <c r="N51" t="s">
+        <v>359</v>
+      </c>
+      <c r="O51" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P51" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>356</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>90</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="K52" t="s">
+        <v>357</v>
+      </c>
+      <c r="N52" t="s">
+        <v>360</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P52" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>364</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>32</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="K53" t="s">
+        <v>372</v>
+      </c>
+      <c r="O53" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P53" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>364</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>33</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="H54" s="3"/>
+      <c r="K54" t="s">
+        <v>9</v>
+      </c>
+      <c r="O54" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P54" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>364</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>33</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="K55" t="s">
+        <v>365</v>
+      </c>
+      <c r="O55" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>370</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>41</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H56" s="3"/>
+      <c r="K56" t="s">
+        <v>9</v>
+      </c>
+      <c r="O56" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>381</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>101</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="K57" t="s">
+        <v>372</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>381</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>79</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="H58" s="3"/>
+      <c r="K58" t="s">
+        <v>372</v>
+      </c>
+      <c r="O58" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>380</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <v>574</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H59" s="3"/>
+      <c r="K59" t="s">
+        <v>379</v>
+      </c>
+      <c r="L59" t="s">
+        <v>377</v>
+      </c>
+      <c r="M59">
+        <v>6</v>
+      </c>
+      <c r="N59" t="s">
+        <v>378</v>
+      </c>
+      <c r="O59" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P59" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="G61" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78366DC7-9A39-E24B-AC3B-88802F01F8CB}">
+  <dimension ref="A1:P318"/>
+  <sheetViews>
+    <sheetView topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="A259" sqref="A259:XFD316"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="55.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2">
@@ -16420,7 +18826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P732"/>
   <sheetViews>

</xml_diff>